<commit_message>
Update mappings & add converter
</commit_message>
<xml_diff>
--- a/data/kode_barang.xlsx
+++ b/data/kode_barang.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CORESTRESS-AI\V2.1 - STABLE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT\Corestress\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053B89C0-92DB-4DBF-9CE5-A22A81067103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07515DBD-B0E3-446D-9953-43A1A39CCA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D33F2AC-AB50-440E-A19D-97662266B360}"/>
   </bookViews>
@@ -797,7 +797,7 @@
   <dimension ref="A1:T81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>